<commit_message>
fixed excel course code
</commit_message>
<xml_diff>
--- a/grades3.xlsx
+++ b/grades3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\liaskentzou\saas25-27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8065005-3BD4-4178-B1CD-A99D19E1B992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D61C7BC-D6BA-4A6F-94DB-46E9988B7AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{721E483D-F02F-DA43-A7B8-6BF48DA94536}"/>
   </bookViews>
@@ -947,10 +947,10 @@
     <t>2024-2025 ΕΑΡ 2025</t>
   </si>
   <si>
-    <t>ΤΕΧΝΗΤΗ ΝΟΗΜΟΣΥΝΗ (3205) 2024-2025 Εαρινή</t>
-  </si>
-  <si>
-    <t>ΤΕΧΝΗΤΗ ΝΟΗΜΟΣΥΝΗ (3205)</t>
+    <t>ΤΕΧΝΗΤΗ ΝΟΗΜΟΣΥΝΗ (3208) 2024-2025 Εαρινή</t>
+  </si>
+  <si>
+    <t>ΤΕΧΝΗΤΗ ΝΟΗΜΟΣΥΝΗ (3208)</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72233FA6-2DFC-D042-BDFC-53B741AB089F}">
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="R93" sqref="R93"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="R83" sqref="R83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>